<commit_message>
Sprint 2 - Dokumentation
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Id</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Testat i testfall…</t>
-  </si>
-  <si>
     <t>Prioritet</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>1a, 1b, 1c</t>
-  </si>
-  <si>
-    <t>Kvalitetskrav</t>
   </si>
   <si>
     <r>
@@ -193,9 +187,6 @@
     <t>Kravspecifikation</t>
   </si>
   <si>
-    <t>Påbörjad</t>
-  </si>
-  <si>
     <t>I 1a läggs bara några element in för att testa funktion/hur man kangöra</t>
   </si>
   <si>
@@ -215,6 +206,69 @@
   </si>
   <si>
     <t>1e</t>
+  </si>
+  <si>
+    <t>Omstrukturera kod. Globala funktioner. Klasser?</t>
+  </si>
+  <si>
+    <t>Klar</t>
+  </si>
+  <si>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>Ladda experimenteditorn från filer</t>
+  </si>
+  <si>
+    <t>1a och 1b var hårdkodade texter i variabler</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Testat i TF</t>
+  </si>
+  <si>
+    <t>3.2b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formatering i textarea. </t>
+  </si>
+  <si>
+    <t>Tab ger inte tab utan förflyttning av focus till Uppdateringsknapp</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>Iframe laddad innan css uppdateras</t>
+  </si>
+  <si>
+    <t>Ibland hinner inte DOMen i iframen ladda innan den försöker stoppa in css-kod vilket gör att all css blir "inherited" från index.htmls style</t>
+  </si>
+  <si>
+    <t>Nytt krav 1g tillagt. Resultat fungerar för det mesta men laddar inte alltid css-kod specifik för iframen</t>
+  </si>
+  <si>
+    <t>Scenario: Logga in</t>
+  </si>
+  <si>
+    <t>Scenario: Spara mall</t>
+  </si>
+  <si>
+    <t>Scenario: Öppna tidigare sparad mall</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>Användarvänligt gränssnitt</t>
   </si>
 </sst>
 </file>
@@ -298,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -314,6 +368,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,10 +661,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <pane ySplit="885" topLeftCell="A16" activePane="bottomLeft"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,16 +674,16 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="76.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="117.42578125" style="10" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -628,33 +696,36 @@
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -662,10 +733,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -673,250 +750,367 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
+      <c r="G8" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="B11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="8">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="1">
-        <v>4</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1">
-        <v>4</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="F24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="8">
         <v>5</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="1">
-        <v>5</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E26" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="F26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="8">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Sprint 3 - Dokumentation
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>Id</t>
   </si>
@@ -269,6 +269,30 @@
   </si>
   <si>
     <t>Användarvänligt gränssnitt</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>Felmeddelande om användrare försöker spara utan att ha loggat in</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Scenario: Skapa användare</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>Scenario: Logga ut</t>
+  </si>
+  <si>
+    <t>Klar/Ej testad</t>
+  </si>
+  <si>
+    <t>Påbörjad</t>
   </si>
 </sst>
 </file>
@@ -661,12 +685,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="885" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="885" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,10 +1029,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>68</v>
+        <v>78</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E32" s="1">
         <v>3</v>
@@ -1016,10 +1043,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E33" s="1">
         <v>3</v>
@@ -1027,84 +1057,120 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E34" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>5</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E39" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>6</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+    <row r="43" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sprint 5 - Dokumentation
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
   <si>
     <t>Id</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Klar/Ej testad</t>
   </si>
   <si>
-    <t>Påbörjad</t>
-  </si>
-  <si>
     <t>4.7</t>
   </si>
   <si>
@@ -310,10 +307,82 @@
     <t>4.9</t>
   </si>
   <si>
-    <t>Fixa gränssnittet för sparningsfunktioner</t>
-  </si>
-  <si>
     <t>Vad/vilka knappar och fält ska synas och vara aktiva när? Spara och visa mall bara aktiva när en användare är inloggad.</t>
+  </si>
+  <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>Grundstruktur-komposition av sida</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>Inte kunna spara mall med samma namn som en som redan finns</t>
+  </si>
+  <si>
+    <t>4.11</t>
+  </si>
+  <si>
+    <t>4.12</t>
+  </si>
+  <si>
+    <t>Se till att bara den som är inloggad får tillgång till spara, visa, ta bort</t>
+  </si>
+  <si>
+    <t>Ändras till 4.12</t>
+  </si>
+  <si>
+    <t>Klar/Ej testat</t>
+  </si>
+  <si>
+    <t>Felmeddelanden vid öppna mall. Måste mallnamn och mallen måste finnas.</t>
+  </si>
+  <si>
+    <t>4.13</t>
+  </si>
+  <si>
+    <t>Se till att meddelanden avseende in-och utloggning ligger i anslutning till inloggning</t>
+  </si>
+  <si>
+    <t>4.14</t>
+  </si>
+  <si>
+    <t>Layouten på ul för visning av sparade mallar</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>Färgval /estetisk utformning- "grundsida"</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>Byt setTimeOut till document.ready i iframeladdningen</t>
+  </si>
+  <si>
+    <t>Kodändringar</t>
+  </si>
+  <si>
+    <t>Användarvänlighet - genomgång</t>
+  </si>
+  <si>
+    <t>4.15</t>
+  </si>
+  <si>
+    <t>Tänk igenom funktionerna visa, öppna och ta bort mall. Bättre o snyggare struktur</t>
+  </si>
+  <si>
+    <t>Presentation av funktionalitet- Vilka val ska vara möjliga vid vilka tillfällen? Var ska de ligga i sidan?</t>
+  </si>
+  <si>
+    <t>Fixa så att önskad funktion enligt 4.9 fungerar.</t>
   </si>
 </sst>
 </file>
@@ -706,12 +775,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="885" activePane="bottomLeft"/>
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="885" topLeftCell="A24" activePane="bottomLeft"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +959,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>43</v>
@@ -904,7 +973,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
@@ -923,7 +992,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>43</v>
@@ -937,7 +1006,7 @@
         <v>44</v>
       </c>
       <c r="E20" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>43</v>
@@ -995,18 +1064,21 @@
         <v>5</v>
       </c>
       <c r="E26" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="4" t="s">
         <v>62</v>
+      </c>
+      <c r="E27" s="1">
+        <v>7</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>63</v>
@@ -1031,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>43</v>
@@ -1099,144 +1171,309 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="8">
-        <v>10</v>
+        <v>99</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="E35" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D36" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D38" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="G38" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="8">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="8">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B44" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="C44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="8">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B46" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G40" s="10" t="s">
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>5</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>6</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="57" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>7</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="E58" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E60" s="1">
         <v>5</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" s="1">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>6</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dokument - tester och uppdateringar
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="143">
   <si>
     <t>Id</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Scenario: Logga ut</t>
   </si>
   <si>
-    <t>Klar/Ej testad</t>
-  </si>
-  <si>
     <t>4.7</t>
   </si>
   <si>
@@ -322,9 +319,6 @@
     <t>7.2</t>
   </si>
   <si>
-    <t>Inte kunna spara mall med samma namn som en som redan finns</t>
-  </si>
-  <si>
     <t>4.11</t>
   </si>
   <si>
@@ -337,12 +331,6 @@
     <t>Ändras till 4.12</t>
   </si>
   <si>
-    <t>Klar/Ej testat</t>
-  </si>
-  <si>
-    <t>Felmeddelanden vid öppna mall. Måste mallnamn och mallen måste finnas.</t>
-  </si>
-  <si>
     <t>4.13</t>
   </si>
   <si>
@@ -383,6 +371,108 @@
   </si>
   <si>
     <t>Fixa så att önskad funktion enligt 4.9 fungerar.</t>
+  </si>
+  <si>
+    <t>4.16</t>
+  </si>
+  <si>
+    <t>Förslag: Tabell med mallnamn kombinerat med möjligheter att ta bort eller visa.</t>
+  </si>
+  <si>
+    <t>4.17</t>
+  </si>
+  <si>
+    <t>Inte kunna ha lösenord '' (tomt fält)</t>
+  </si>
+  <si>
+    <t>Upptäckt i testfall 7</t>
+  </si>
+  <si>
+    <t>4.18</t>
+  </si>
+  <si>
+    <t>Specificerade felmeddelande som anger vilket fel som gjorts</t>
+  </si>
+  <si>
+    <t>Specificerat felmeddelande om användaren inte finns registrerad</t>
+  </si>
+  <si>
+    <t>Se över när det ska stå vem som är inloggad. Meddelandet försvinner när användaren gör något annat som skapar ett meddelande.</t>
+  </si>
+  <si>
+    <t>Meddelande till användare som försöker logga ut när han inte är inloggad</t>
+  </si>
+  <si>
+    <t>Upptäckt i testfall 8. Felmeddelande visas som säger att lösenordet inte stämmer med användaren.</t>
+  </si>
+  <si>
+    <t>När användare väljer att spara en mall med ett namn som redan finns visas ett meddelande som meddelar att en mall med namnet existerar och en fråga om han vill ersätta den.</t>
+  </si>
+  <si>
+    <t>4.19</t>
+  </si>
+  <si>
+    <t>Om ny användare loggar in på samma dator ska defaultmallar visas och inte en som valts av tidigare användare</t>
+  </si>
+  <si>
+    <t>4.20</t>
+  </si>
+  <si>
+    <t>4.21</t>
+  </si>
+  <si>
+    <t>Ta bort tidigare felmeddelanden när en ny mall öppnats</t>
+  </si>
+  <si>
+    <t>Se över visafunktionen. Inte bara skriva ut mallnamn. Se även 4.9</t>
+  </si>
+  <si>
+    <t>En mall som tas bort ska även tas bort från listan på befintliga mallar (under Visa)</t>
+  </si>
+  <si>
+    <t>4.22</t>
+  </si>
+  <si>
+    <t>När inget mallnamn angetts när användaren trcker på Ta bort bör meddelandet säga att mallen bör anges och inte att det inte finns någon mall med namnet *tomrum'</t>
+  </si>
+  <si>
+    <t>4.23</t>
+  </si>
+  <si>
+    <t>4.24</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>Id 4.17-4.25 tillkom i samband med test 2014-05-22</t>
+  </si>
+  <si>
+    <t>Sprint6</t>
+  </si>
+  <si>
+    <t>1-, 11, 12</t>
+  </si>
+  <si>
+    <t>Felmeddelanden vid öppna mall. Måste ange mallnamn och mallen måste finnas.</t>
+  </si>
+  <si>
+    <t>10, 11, 12</t>
+  </si>
+  <si>
+    <t>Är nog inte så vanligt. Låg rioritering därför</t>
+  </si>
+  <si>
+    <t>Klar/ej test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    </t>
+  </si>
+  <si>
+    <t>Reserv Sprint 6</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
   </si>
 </sst>
 </file>
@@ -446,12 +536,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -466,23 +568,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,6 +584,41 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,56 +900,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="885" topLeftCell="A24" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="705" topLeftCell="A28" activePane="bottomLeft"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="76.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="117.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="117.42578125" style="6" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -832,16 +957,16 @@
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="9">
         <v>1</v>
       </c>
     </row>
@@ -849,16 +974,16 @@
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="10">
         <v>2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="9">
         <v>1</v>
       </c>
     </row>
@@ -866,19 +991,19 @@
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="10">
         <v>3</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="9">
         <v>1</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -886,13 +1011,17 @@
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="1">
+      <c r="C9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="12">
         <v>4</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -900,13 +1029,17 @@
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="1">
+      <c r="C10" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="12">
         <v>4</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -914,16 +1047,17 @@
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="E11" s="9"/>
+      <c r="G11" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -931,23 +1065,23 @@
       <c r="A12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
+      <c r="B13" s="19"/>
     </row>
     <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -955,8 +1089,11 @@
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="18" t="s">
         <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E16" s="1">
         <v>6</v>
@@ -969,8 +1106,11 @@
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="18" t="s">
         <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E17" s="1">
         <v>6</v>
@@ -980,7 +1120,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -988,8 +1128,11 @@
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="18" t="s">
         <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
@@ -1002,8 +1145,11 @@
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="18" t="s">
         <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
@@ -1013,467 +1159,652 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="10">
         <v>4</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E25" s="9">
         <v>2</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D27" s="10">
         <v>5</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E27" s="9">
         <v>2</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E28" s="1">
         <v>7</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G28" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D30" s="10">
         <v>6</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E30" s="9">
         <v>2</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="18"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="18"/>
+    </row>
+    <row r="33" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>4</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="8">
-        <v>7</v>
-      </c>
-      <c r="E32" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="8">
-        <v>8</v>
-      </c>
-      <c r="E33" s="1">
-        <v>3</v>
+      <c r="G33" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="8">
-        <v>9</v>
-      </c>
-      <c r="E34" s="1">
+        <v>77</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="10">
+        <v>7</v>
+      </c>
+      <c r="E34" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>100</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="11"/>
       <c r="E35" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="8">
-        <v>10</v>
+        <v>114</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="E36" s="1">
+        <v>7</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="10">
+        <v>8</v>
+      </c>
+      <c r="E38" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="8">
-        <v>10</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="1">
+        <v>9</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="8">
-        <v>11</v>
+        <v>123</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E40" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" s="8">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1">
-        <v>5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" s="1">
+        <v>9</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="1">
+        <v>79</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="10">
+        <v>9</v>
+      </c>
+      <c r="E43" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>85</v>
+        <v>95</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="8">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="E44" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="10">
+        <v>10</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="G49" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="10">
+        <v>11</v>
+      </c>
+      <c r="E51" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="10">
+        <v>11</v>
+      </c>
+      <c r="E52" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="10">
+        <v>13</v>
+      </c>
+      <c r="E55" s="9">
+        <v>3</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E56" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E57" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" s="10">
+        <v>12</v>
+      </c>
+      <c r="E59" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E60" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" s="1">
+        <v>7</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E63" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E64" s="1">
+        <v>7</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>5</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B68" s="15"/>
+    </row>
+    <row r="69" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>6</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E71" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B72" s="15"/>
+    </row>
+    <row r="74" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>7</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E76" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="B78" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E78" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E46" s="1">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="1">
+      <c r="B88" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E48" s="1">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>5</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E50" s="1">
+      <c r="B89" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>6</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E54" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-    </row>
-    <row r="57" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>7</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E58" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E59" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E61" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B73" s="1" t="s">
+      <c r="B90" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sprint 6 - Dokumentation
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="146">
   <si>
     <t>Id</t>
   </si>
@@ -448,9 +448,6 @@
     <t>Id 4.17-4.25 tillkom i samband med test 2014-05-22</t>
   </si>
   <si>
-    <t>Sprint6</t>
-  </si>
-  <si>
     <t>1-, 11, 12</t>
   </si>
   <si>
@@ -472,7 +469,19 @@
     <t>Reserv Sprint 6</t>
   </si>
   <si>
-    <t>Sprint 6</t>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Iframe anpassar höjd efter innehåll</t>
+  </si>
+  <si>
+    <t>Sprint7</t>
+  </si>
+  <si>
+    <t>Det bör inte längre vara ett möjligt val att logga ut när man inte är inloggad.</t>
+  </si>
+  <si>
+    <t>Klar/Ej test</t>
   </si>
 </sst>
 </file>
@@ -568,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -618,6 +627,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -900,12 +912,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="705" topLeftCell="A28" activePane="bottomLeft"/>
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="885" topLeftCell="A59" activePane="bottomLeft"/>
+      <selection activeCell="A61" sqref="A61:B61"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,151 +1019,149 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12">
-        <v>4</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="12">
         <v>4</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="12">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="G11" s="6" t="s">
+      <c r="E12" s="9"/>
+      <c r="G12" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B13" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E16" s="1">
-        <v>6</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" s="1">
+        <v>35</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="12">
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="12">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="1">
-        <v>6</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E20" s="1">
+        <v>37</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12">
         <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1159,347 +1169,349 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="12">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
     </row>
-    <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B26" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D26" s="10">
         <v>4</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E26" s="9">
         <v>2</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B28" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D28" s="10">
         <v>5</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E28" s="9">
         <v>2</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E29" s="1">
         <v>7</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D31" s="10">
         <v>6</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E31" s="9">
         <v>2</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
     </row>
-    <row r="33" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="18"/>
+    </row>
+    <row r="34" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>4</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B35" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D35" s="10">
         <v>7</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E35" s="9">
         <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="1">
-        <v>6</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D36" s="11"/>
       <c r="E36" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="1">
+        <v>9</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B39" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D39" s="10">
         <v>8</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E40" s="1">
         <v>9</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="1">
-        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E42" s="1">
         <v>9</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="G42" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B44" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D44" s="10">
         <v>9</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E44" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="1">
+      <c r="C45" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E46" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="G46" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B48" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D48" s="10">
         <v>10</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E48" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="1">
+      <c r="C49" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B50" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E49" s="9"/>
-      <c r="G49" s="6" t="s">
+      <c r="D50" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="G50" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B52" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="10">
-        <v>11</v>
-      </c>
-      <c r="E51" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>136</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>55</v>
@@ -1508,303 +1520,324 @@
         <v>11</v>
       </c>
       <c r="E52" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="10">
+        <v>11</v>
+      </c>
+      <c r="E53" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B54" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="1">
+      <c r="C54" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="13"/>
+      <c r="E54" s="12">
         <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="10">
-        <v>13</v>
-      </c>
-      <c r="E55" s="9">
-        <v>3</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="10">
+        <v>13</v>
+      </c>
+      <c r="E56" s="9">
+        <v>3</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="E56" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="E57" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="58" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B60" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C60" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D60" s="10">
         <v>12</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E60" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E60" s="1">
+      <c r="C61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B62" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E61" s="1">
+      <c r="C62" s="6"/>
+      <c r="E62" s="1">
         <v>7</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="G62" s="6" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="E62" s="9">
-        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E63" s="1">
-        <v>6</v>
+        <v>92</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" s="9">
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E64" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B65" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E65" s="1">
         <v>7</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="G65" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B65" s="8"/>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="8"/>
+    </row>
+    <row r="68" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>5</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B68" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E68" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B68" s="15"/>
-    </row>
-    <row r="69" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+    <row r="69" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="15"/>
+    </row>
+    <row r="70" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>6</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B70" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="6" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E71" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E72" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B72" s="15"/>
-    </row>
-    <row r="74" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="73" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B73" s="15"/>
+    </row>
+    <row r="75" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>7</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B75" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B76" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E75" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="C76" s="1" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="E76" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E77" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B78" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E77" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>104</v>
+      <c r="C78" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="E78" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B79" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E79" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E80" s="1">
         <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B91" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sprint 7-Dokumentation. Kod i version 140601-3
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="172">
   <si>
     <t>Id</t>
   </si>
@@ -370,9 +370,6 @@
     <t>Inte kunna ha lösenord '' (tomt fält)</t>
   </si>
   <si>
-    <t>Upptäckt i testfall 7</t>
-  </si>
-  <si>
     <t>4.18</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>Meddelande till användare som försöker logga ut när han inte är inloggad</t>
   </si>
   <si>
-    <t>Upptäckt i testfall 8. Felmeddelande visas som säger att lösenordet inte stämmer med användaren.</t>
-  </si>
-  <si>
     <t>När användare väljer att spara en mall med ett namn som redan finns visas ett meddelande som meddelar att en mall med namnet existerar och en fråga om han vill ersätta den.</t>
   </si>
   <si>
@@ -418,9 +412,6 @@
     <t>4.22</t>
   </si>
   <si>
-    <t>När inget mallnamn angetts när användaren trcker på Ta bort bör meddelandet säga att mallen bör anges och inte att det inte finns någon mall med namnet *tomrum'</t>
-  </si>
-  <si>
     <t>4.23</t>
   </si>
   <si>
@@ -466,9 +457,6 @@
     <t>Det bör inte längre vara ett möjligt val att logga ut när man inte är inloggad.</t>
   </si>
   <si>
-    <t>Klar/Ej test</t>
-  </si>
-  <si>
     <t>Optimera/omstrukturera inloggning</t>
   </si>
   <si>
@@ -524,6 +512,54 @@
   </si>
   <si>
     <t>Workshop3</t>
+  </si>
+  <si>
+    <t>Har lagt in hjälptext som byts mot mallhanteringsruta vid inloggning</t>
+  </si>
+  <si>
+    <t>4.28</t>
+  </si>
+  <si>
+    <t>4.29</t>
+  </si>
+  <si>
+    <t>4.30</t>
+  </si>
+  <si>
+    <t>Töm input om man matat in namnet på en mall som inte finns</t>
+  </si>
+  <si>
+    <t>Upptäckt i testfall 11 Test 2014-05-30</t>
+  </si>
+  <si>
+    <t>4.31</t>
+  </si>
+  <si>
+    <t>Meddelanden ska raderas vid utloggning och inte ligga kvar till nästa som loggar in</t>
+  </si>
+  <si>
+    <t>Flytta funktionaliteten från från knapp till faktisk utloggning, se 140528 Användartest</t>
+  </si>
+  <si>
+    <t>Radera visade mallar och återställ knapp vid utloggning, se 140528 Användartest</t>
+  </si>
+  <si>
+    <t>Upptäckt i testfall 7  Test 140522</t>
+  </si>
+  <si>
+    <t>Upptäckt i testfall 8 Test 140522. Felmeddelande visas som säger att lösenordet inte stämmer med användaren.</t>
+  </si>
+  <si>
+    <t>7 Test 140601</t>
+  </si>
+  <si>
+    <t>8 Test 140601</t>
+  </si>
+  <si>
+    <t>När inget mallnamn angetts när användaren trycker på Ta bort bör meddelandet säga att mallen bör anges och inte att det inte finns någon mall med namnet *tomrum'</t>
+  </si>
+  <si>
+    <t>Upptäcktes vid test 2024-06-01</t>
   </si>
 </sst>
 </file>
@@ -962,12 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="885" topLeftCell="A4" activePane="bottomLeft"/>
-      <selection activeCell="B65" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +1011,7 @@
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="117.42578125" style="6" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1071,10 +1105,10 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="1">
@@ -1089,7 +1123,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="12">
@@ -1107,7 +1141,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="12">
@@ -1167,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="12">
@@ -1185,7 +1219,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="12">
@@ -1208,7 +1242,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="12">
@@ -1226,7 +1260,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="12">
@@ -1254,7 +1288,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>25</v>
@@ -1279,7 +1313,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>27</v>
@@ -1299,7 +1333,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>57</v>
@@ -1318,7 +1352,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>29</v>
@@ -1350,7 +1384,7 @@
         <v>30</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1382,21 +1416,27 @@
         <v>8</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="C37" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="9">
         <v>9</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1421,24 +1461,30 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="1">
+        <v>114</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="9">
         <v>9</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E41" s="1">
         <v>8</v>
@@ -1446,16 +1492,16 @@
     </row>
     <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E42" s="1">
         <v>9</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1475,491 +1521,574 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="12">
+      <c r="C45" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="10">
+        <v>14</v>
+      </c>
+      <c r="E45" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B46" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="9">
+        <v>9</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="10">
+        <v>2</v>
+      </c>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="10">
+        <v>22</v>
+      </c>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="10">
+        <v>23</v>
+      </c>
+      <c r="E49" s="9">
+        <v>7</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="24"/>
+      <c r="D50" s="11"/>
+      <c r="G50" s="25"/>
+    </row>
+    <row r="51" spans="1:7" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="24"/>
+      <c r="D51" s="11"/>
+      <c r="G51" s="25"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="10">
+        <v>10</v>
+      </c>
+      <c r="E52" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E46" s="1">
-        <v>9</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="10">
-        <v>10</v>
-      </c>
-      <c r="E49" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="1">
+      <c r="C53" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B54" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E51" s="9"/>
-      <c r="G51" s="6" t="s">
+      <c r="C54" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E54" s="9"/>
+      <c r="G54" s="6" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="10">
-        <v>11</v>
-      </c>
-      <c r="E54" s="9">
-        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="10">
+        <v>11</v>
+      </c>
+      <c r="E57" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="10">
+      <c r="B58" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="10">
         <v>11</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E58" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="12">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="10">
+        <v>15</v>
+      </c>
+      <c r="E59" s="9">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="B57" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="23">
+    <row r="60" spans="1:7" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="E60" s="23">
         <v>8</v>
       </c>
-      <c r="G57" s="25"/>
-    </row>
-    <row r="58" spans="1:7" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="24"/>
-      <c r="D58" s="11"/>
-      <c r="G58" s="25"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D60" s="10">
-        <v>13</v>
-      </c>
-      <c r="E60" s="9">
-        <v>3</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E61" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" s="1">
-        <v>9</v>
-      </c>
+      <c r="G60" s="25"/>
+    </row>
+    <row r="61" spans="1:7" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D61" s="10">
+        <v>24</v>
+      </c>
+      <c r="E61" s="9">
+        <v>7</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="24"/>
+      <c r="D62" s="11"/>
+      <c r="G62" s="25"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D64" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E64" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G64" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B65" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="12">
-        <v>6</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C66" s="6"/>
+        <v>170</v>
+      </c>
       <c r="E66" s="1">
-        <v>7</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B67" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E68" s="1">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D68" s="10">
+        <v>12</v>
+      </c>
+      <c r="E68" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E69" s="1">
-        <v>7</v>
+        <v>92</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D69" s="13"/>
+      <c r="E69" s="12">
+        <v>6</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="8"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="6"/>
       <c r="E70" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="G70" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E71" s="9">
         <v>5</v>
       </c>
-      <c r="B71" s="15" t="s">
+    </row>
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E72" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E73" s="1">
+        <v>7</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>5</v>
+      </c>
+      <c r="B75" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E75" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B72" s="15"/>
-    </row>
-    <row r="73" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>6</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E74" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E75" s="1">
-        <v>7</v>
-      </c>
+    <row r="76" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B76" s="15"/>
     </row>
     <row r="77" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
+        <v>6</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E78" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E79" s="1">
         <v>7</v>
       </c>
-      <c r="B77" s="15" t="s">
+    </row>
+    <row r="81" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>7</v>
+      </c>
+      <c r="B81" s="15" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E78" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E79" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E80" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E81" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>145</v>
+        <v>83</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="E82" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E83" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E84" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E85" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E86" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E83" s="1">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E87" s="1">
         <v>9</v>
       </c>
-      <c r="G83" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="G87" s="22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>8</v>
       </c>
-      <c r="B85" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E86" s="1">
+      <c r="B89" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E90" s="1">
         <v>9</v>
       </c>
-      <c r="G86" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>7</v>
+      <c r="G90" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B97" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>